<commit_message>
Added some changes to quantile_calculations
</commit_message>
<xml_diff>
--- a/datasets/NADPARK_differential/mmc6.xlsx
+++ b/datasets/NADPARK_differential/mmc6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hvl365-my.sharepoint.com/personal/585090_stud_hvl_no/Documents/Masteroppgave/Kode/parkinsonbayes/datasets/NADPARK_differential/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="8_{5920782C-FFA2-48E3-BD04-EBDFFDD513B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E5C25F1-EA93-4AF8-9E96-78015936A7EA}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{5920782C-FFA2-48E3-BD04-EBDFFDD513B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C2CC725-15F2-458D-AA8C-946B869FA2E6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="162">
   <si>
     <r>
       <t>Figure 1D: Relative total NAD levels normalized to ATP-</t>
@@ -668,6 +668,15 @@
   <si>
     <t>Diff</t>
   </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>Muscle NAAD</t>
+  </si>
+  <si>
+    <t>PBMCs</t>
+  </si>
 </sst>
 </file>
 
@@ -1042,7 +1051,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1271,32 +1280,44 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1307,17 +1328,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1631,7 +1652,7 @@
   <dimension ref="B2:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F20"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,91 +1701,112 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="3">
-        <v>0.30522250000000001</v>
+        <v>0.30607499999999999</v>
       </c>
       <c r="E5" s="3">
-        <v>0.4326197</v>
+        <v>0.12742249999999999</v>
       </c>
       <c r="F5">
         <f>E5-D5</f>
-        <v>0.12739719999999999</v>
+        <v>-0.17865249999999999</v>
       </c>
       <c r="G5">
         <f>D5/E5</f>
-        <v>0.70552150075458886</v>
+        <v>2.4020483038709806</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="48" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C6" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="3">
-        <v>0.30607499999999999</v>
+        <v>0.34194639999999998</v>
       </c>
       <c r="E6" s="3">
-        <v>0.12742249999999999</v>
+        <v>0.22280349999999999</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F32" si="0">E6-D6</f>
-        <v>-0.17865249999999999</v>
+        <f>E6-D6</f>
+        <v>-0.1191429</v>
       </c>
       <c r="G6">
         <f>D6/E6</f>
-        <v>2.4020483038709806</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>1.5347442926165882</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="101" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="101" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="102">
+        <v>0.2809104</v>
+      </c>
+      <c r="E7" s="102">
+        <v>0.18809429999999999</v>
+      </c>
+      <c r="F7">
+        <f>E7-D7</f>
+        <v>-9.2816100000000012E-2</v>
+      </c>
+      <c r="G7">
+        <f>D7/E7</f>
+        <v>1.4934551445737592</v>
+      </c>
+    </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="48" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C8" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="3">
-        <v>0.24157619999999999</v>
+        <v>0.21947939999999999</v>
       </c>
       <c r="E8" s="3">
-        <v>0.25536759999999997</v>
+        <v>0.1587538</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
-        <v>1.3791399999999981E-2</v>
+        <f>E8-D8</f>
+        <v>-6.0725599999999991E-2</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G32" si="1">D8/E8</f>
-        <v>0.94599393188485936</v>
+        <f>D8/E8</f>
+        <v>1.3825143083189189</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="47" t="s">
-        <v>2</v>
+        <v>31</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="D9" s="3">
-        <v>0.25199769999999999</v>
+        <v>0.36078189999999999</v>
       </c>
       <c r="E9" s="3">
-        <v>0.25020120000000001</v>
+        <v>0.32562190000000002</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
-        <v>-1.7964999999999787E-3</v>
+        <f>E9-D9</f>
+        <v>-3.5159999999999969E-2</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
-        <v>1.0071802213578511</v>
+        <f>D9/E9</f>
+        <v>1.107977995337537</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -1781,188 +1823,188 @@
         <v>0.60721219999999998</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f>E10-D10</f>
         <v>-3.1334300000000037E-2</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f>D10/E10</f>
         <v>1.0516035415625709</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="48" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C11" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="3">
-        <v>0.48137869999999999</v>
+        <v>0.23669219999999999</v>
       </c>
       <c r="E11" s="3">
-        <v>0.4647715</v>
+        <v>0.21753140000000001</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
-        <v>-1.6607199999999989E-2</v>
+        <f>E11-D11</f>
+        <v>-1.9160799999999978E-2</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
-        <v>1.0357319672139966</v>
+        <f>D11/E11</f>
+        <v>1.0880829158457124</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="3">
-        <v>0.38636379999999998</v>
+        <v>0.48137869999999999</v>
       </c>
       <c r="E12" s="3">
-        <v>0.38053769999999998</v>
+        <v>0.4647715</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
-        <v>-5.8261000000000007E-3</v>
+        <f>E12-D12</f>
+        <v>-1.6607199999999989E-2</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
-        <v>1.0153101782031058</v>
+        <f>D12/E12</f>
+        <v>1.0357319672139966</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="3">
-        <v>0.21947939999999999</v>
+        <v>0.38636379999999998</v>
       </c>
       <c r="E13" s="3">
-        <v>0.1587538</v>
+        <v>0.38053769999999998</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
-        <v>-6.0725599999999991E-2</v>
+        <f>E13-D13</f>
+        <v>-5.8261000000000007E-3</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
-        <v>1.3825143083189189</v>
+        <f>D13/E13</f>
+        <v>1.0153101782031058</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="48" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C14" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="3">
-        <v>0.34194639999999998</v>
+        <v>0.21959039999999999</v>
       </c>
       <c r="E14" s="3">
-        <v>0.22280349999999999</v>
+        <v>0.21698980000000001</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
-        <v>-0.1191429</v>
+        <f>E14-D14</f>
+        <v>-2.6005999999999807E-3</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
-        <v>1.5347442926165882</v>
+        <f>D14/E14</f>
+        <v>1.0119848951425365</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="48" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C15" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="3">
-        <v>0.2421827</v>
+        <v>0.25199769999999999</v>
       </c>
       <c r="E15" s="3">
-        <v>0.351962</v>
+        <v>0.25020120000000001</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
-        <v>0.1097793</v>
+        <f>E15-D15</f>
+        <v>-1.7964999999999787E-3</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
-        <v>0.68809331689216446</v>
+        <f>D15/E15</f>
+        <v>1.0071802213578511</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="47" t="s">
-        <v>2</v>
+        <v>28</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="D16" s="3">
-        <v>0.22928509999999999</v>
+        <v>0.33677810000000002</v>
       </c>
       <c r="E16" s="3">
-        <v>0.28075850000000002</v>
+        <v>0.34204390000000001</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
-        <v>5.147340000000003E-2</v>
+        <f>E16-D16</f>
+        <v>5.2657999999999872E-3</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
-        <v>0.81666307520520298</v>
+        <f>D16/E16</f>
+        <v>0.98460490013124047</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="48" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C17" s="47" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="3">
-        <v>0.21959039999999999</v>
+        <v>0.24157619999999999</v>
       </c>
       <c r="E17" s="3">
-        <v>0.21698980000000001</v>
+        <v>0.25536759999999997</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
-        <v>-2.6005999999999807E-3</v>
+        <f>E17-D17</f>
+        <v>1.3791399999999981E-2</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
-        <v>1.0119848951425365</v>
+        <f>D17/E17</f>
+        <v>0.94599393188485936</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="C18" s="48" t="s">
+        <v>3</v>
       </c>
       <c r="D18" s="3">
-        <v>0.23669219999999999</v>
+        <v>0.29680279999999998</v>
       </c>
       <c r="E18" s="3">
-        <v>0.21753140000000001</v>
+        <v>0.3143552</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
-        <v>-1.9160799999999978E-2</v>
+        <f>E18-D18</f>
+        <v>1.7552400000000024E-2</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
-        <v>1.0880829158457124</v>
+        <f>D18/E18</f>
+        <v>0.94416379942180051</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -1979,122 +2021,122 @@
         <v>0.22621910000000001</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f>E19-D19</f>
         <v>3.6556300000000014E-2</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f>D19/E19</f>
         <v>0.83840312334369638</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="48" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C20" s="48" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="3">
-        <v>0.2809104</v>
+        <v>0.31188660000000001</v>
       </c>
       <c r="E20" s="3">
-        <v>0.18809429999999999</v>
+        <v>0.35785289999999997</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
-        <v>-9.2816100000000012E-2</v>
+        <f>E20-D20</f>
+        <v>4.596629999999996E-2</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
-        <v>1.4934551445737592</v>
+        <f>D20/E20</f>
+        <v>0.87154973454176299</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="48" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C21" s="48" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="3">
-        <v>0.1999676</v>
+        <v>0.33392729999999998</v>
       </c>
       <c r="E21" s="3">
-        <v>0.30869970000000002</v>
+        <v>0.38342680000000001</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
-        <v>0.10873210000000003</v>
+        <f>E21-D21</f>
+        <v>4.949950000000003E-2</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
-        <v>0.64777387214823978</v>
+        <f>D21/E21</f>
+        <v>0.87090234694079804</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="48" t="s">
-        <v>3</v>
+        <v>17</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>2</v>
       </c>
       <c r="D22" s="3">
-        <v>0.2331281</v>
+        <v>0.22928509999999999</v>
       </c>
       <c r="E22" s="3">
-        <v>0.33454040000000002</v>
+        <v>0.28075850000000002</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
-        <v>0.10141230000000001</v>
+        <f>E22-D22</f>
+        <v>5.147340000000003E-2</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
-        <v>0.69686082757119916</v>
+        <f>D22/E22</f>
+        <v>0.81666307520520298</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="48" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C23" s="48" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="3">
-        <v>0.30449910000000002</v>
+        <v>0.29977300000000001</v>
       </c>
       <c r="E23" s="3">
-        <v>0.5617335</v>
+        <v>0.37562909999999999</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
-        <v>0.25723439999999997</v>
+        <f>E23-D23</f>
+        <v>7.5856099999999982E-2</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
-        <v>0.54207039459102946</v>
+        <f>D23/E23</f>
+        <v>0.79805584817576702</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="48" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C24" s="48" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="3">
-        <v>0.31188660000000001</v>
+        <v>0.2331281</v>
       </c>
       <c r="E24" s="3">
-        <v>0.35785289999999997</v>
+        <v>0.33454040000000002</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
-        <v>4.596629999999996E-2</v>
+        <f>E24-D24</f>
+        <v>0.10141230000000001</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
-        <v>0.87154973454176299</v>
+        <f>D24/E24</f>
+        <v>0.69686082757119916</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -2111,169 +2153,156 @@
         <v>0.42068840000000002</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f>E25-D25</f>
         <v>0.10778219999999999</v>
       </c>
       <c r="G25">
-        <f t="shared" si="1"/>
+        <f>D25/E25</f>
         <v>0.7437956454230733</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="48" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C26" s="48" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="3">
-        <v>0.23489070000000001</v>
+        <v>0.1999676</v>
       </c>
       <c r="E26" s="3">
-        <v>0.34709190000000001</v>
+        <v>0.30869970000000002</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
-        <v>0.1122012</v>
+        <f>E26-D26</f>
+        <v>0.10873210000000003</v>
       </c>
       <c r="G26">
-        <f t="shared" si="1"/>
-        <v>0.67673921517615365</v>
+        <f>D26/E26</f>
+        <v>0.64777387214823978</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="48" t="s">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>2</v>
       </c>
       <c r="D27" s="3">
-        <v>0.24444089999999999</v>
+        <v>0.2421827</v>
       </c>
       <c r="E27" s="3">
-        <v>0.50193779999999999</v>
+        <v>0.351962</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
-        <v>0.25749690000000003</v>
+        <f>E27-D27</f>
+        <v>0.1097793</v>
       </c>
       <c r="G27">
-        <f t="shared" si="1"/>
-        <v>0.48699440448597414</v>
+        <f>D27/E27</f>
+        <v>0.68809331689216446</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C28" s="48" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="3">
-        <v>0.33677810000000002</v>
+        <v>0.23489070000000001</v>
       </c>
       <c r="E28" s="3">
-        <v>0.34204390000000001</v>
+        <v>0.34709190000000001</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
-        <v>5.2657999999999872E-3</v>
+        <f>E28-D28</f>
+        <v>0.1122012</v>
       </c>
       <c r="G28">
-        <f t="shared" si="1"/>
-        <v>0.98460490013124047</v>
+        <f>D28/E28</f>
+        <v>0.67673921517615365</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="48" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>2</v>
       </c>
       <c r="D29" s="3">
-        <v>0.33392729999999998</v>
+        <v>0.30522250000000001</v>
       </c>
       <c r="E29" s="3">
-        <v>0.38342680000000001</v>
+        <v>0.4326197</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
-        <v>4.949950000000003E-2</v>
+        <f>E29-D29</f>
+        <v>0.12739719999999999</v>
       </c>
       <c r="G29">
-        <f t="shared" si="1"/>
-        <v>0.87090234694079804</v>
+        <f>D29/E29</f>
+        <v>0.70552150075458886</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="48" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C30" s="48" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="3">
-        <v>0.29977300000000001</v>
+        <v>0.30449910000000002</v>
       </c>
       <c r="E30" s="3">
-        <v>0.37562909999999999</v>
+        <v>0.5617335</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
-        <v>7.5856099999999982E-2</v>
+        <f>E30-D30</f>
+        <v>0.25723439999999997</v>
       </c>
       <c r="G30">
-        <f t="shared" si="1"/>
-        <v>0.79805584817576702</v>
+        <f>D30/E30</f>
+        <v>0.54207039459102946</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="48" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C31" s="48" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="3">
-        <v>0.36078189999999999</v>
+        <v>0.24444089999999999</v>
       </c>
       <c r="E31" s="3">
-        <v>0.32562190000000002</v>
+        <v>0.50193779999999999</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
-        <v>-3.5159999999999969E-2</v>
+        <f>E31-D31</f>
+        <v>0.25749690000000003</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
-        <v>1.107977995337537</v>
+        <f>D31/E31</f>
+        <v>0.48699440448597414</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="3">
-        <v>0.29680279999999998</v>
-      </c>
-      <c r="E32" s="3">
-        <v>0.3143552</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="0"/>
-        <v>1.7552400000000024E-2</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="1"/>
-        <v>0.94416379942180051</v>
-      </c>
+      <c r="B32" s="100"/>
+      <c r="C32" s="100"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:G32">
+    <sortCondition ref="F32"/>
+  </sortState>
   <mergeCells count="2">
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B2:E2"/>
@@ -4560,8 +4589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:V66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37:E66"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E66" sqref="E37:E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6514,369 +6543,663 @@
         <v>7.2844800000000003</v>
       </c>
     </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C36" s="1">
+        <v>0.14416999999999999</v>
+      </c>
+      <c r="D36" s="1">
+        <v>8.5860000000000006E-2</v>
+      </c>
+      <c r="E36">
+        <f>D36-C36</f>
+        <v>-5.8309999999999987E-2</v>
+      </c>
+      <c r="I36">
+        <v>0.88570000000000004</v>
+      </c>
+      <c r="J36">
+        <v>0.15307999999999999</v>
+      </c>
+      <c r="K36">
+        <f>J36-I36</f>
+        <v>-0.73262000000000005</v>
+      </c>
+    </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
-        <v>0.14416999999999999</v>
+        <v>9.2149999999999996E-2</v>
       </c>
       <c r="D37" s="1">
-        <v>8.5860000000000006E-2</v>
+        <v>4.9630000000000001E-2</v>
       </c>
       <c r="E37">
         <f>D37-C37</f>
-        <v>-5.8309999999999987E-2</v>
+        <v>-4.2519999999999995E-2</v>
+      </c>
+      <c r="I37">
+        <v>0.71394999999999997</v>
+      </c>
+      <c r="J37">
+        <v>0.36658000000000002</v>
+      </c>
+      <c r="K37">
+        <f>J37-I37</f>
+        <v>-0.34736999999999996</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
-        <v>9.2149999999999996E-2</v>
+        <v>8.4089999999999998E-2</v>
       </c>
       <c r="D38" s="1">
-        <v>4.9630000000000001E-2</v>
+        <v>5.4530000000000002E-2</v>
       </c>
       <c r="E38">
         <f>D38-C38</f>
-        <v>-4.2519999999999995E-2</v>
+        <v>-2.9559999999999996E-2</v>
+      </c>
+      <c r="I38">
+        <v>0.46134999999999998</v>
+      </c>
+      <c r="J38">
+        <v>0.29488999999999999</v>
+      </c>
+      <c r="K38">
+        <f>J38-I38</f>
+        <v>-0.16646</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
-        <v>8.4089999999999998E-2</v>
+        <v>0.15690000000000001</v>
       </c>
       <c r="D39" s="1">
-        <v>5.4530000000000002E-2</v>
+        <v>0.13062000000000001</v>
       </c>
       <c r="E39">
         <f>D39-C39</f>
-        <v>-2.9559999999999996E-2</v>
+        <v>-2.6279999999999998E-2</v>
+      </c>
+      <c r="I39">
+        <v>0.18304999999999999</v>
+      </c>
+      <c r="J39">
+        <v>0.10818999999999999</v>
+      </c>
+      <c r="K39">
+        <f>J39-I39</f>
+        <v>-7.4859999999999996E-2</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
-        <v>0.15690000000000001</v>
+        <v>0.10892</v>
       </c>
       <c r="D40" s="1">
-        <v>0.13062000000000001</v>
+        <v>8.7529999999999997E-2</v>
       </c>
       <c r="E40">
         <f>D40-C40</f>
-        <v>-2.6279999999999998E-2</v>
+        <v>-2.1390000000000006E-2</v>
+      </c>
+      <c r="I40">
+        <v>0.17591999999999999</v>
+      </c>
+      <c r="J40">
+        <v>0.11019</v>
+      </c>
+      <c r="K40">
+        <f>J40-I40</f>
+        <v>-6.5729999999999997E-2</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
-        <v>0.10892</v>
+        <v>3.7960000000000001E-2</v>
       </c>
       <c r="D41" s="1">
-        <v>8.7529999999999997E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="E41">
         <f>D41-C41</f>
-        <v>-2.1390000000000006E-2</v>
+        <v>-3.9599999999999982E-3</v>
+      </c>
+      <c r="I41">
+        <v>0.22772999999999999</v>
+      </c>
+      <c r="J41">
+        <v>0.17598</v>
+      </c>
+      <c r="K41">
+        <f>J41-I41</f>
+        <v>-5.174999999999999E-2</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
-        <v>3.7960000000000001E-2</v>
+        <v>9.7900000000000001E-2</v>
       </c>
       <c r="D42" s="1">
-        <v>3.4000000000000002E-2</v>
+        <v>9.5259999999999997E-2</v>
       </c>
       <c r="E42">
         <f>D42-C42</f>
-        <v>-3.9599999999999982E-3</v>
+        <v>-2.6400000000000035E-3</v>
+      </c>
+      <c r="I42">
+        <v>0.31950000000000001</v>
+      </c>
+      <c r="J42">
+        <v>0.27535999999999999</v>
+      </c>
+      <c r="K42">
+        <f>J42-I42</f>
+        <v>-4.4140000000000013E-2</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
-        <v>9.7900000000000001E-2</v>
+        <v>0.15583</v>
       </c>
       <c r="D43" s="1">
-        <v>9.5259999999999997E-2</v>
+        <v>0.15583</v>
       </c>
       <c r="E43">
         <f>D43-C43</f>
-        <v>-2.6400000000000035E-3</v>
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0.18472</v>
+      </c>
+      <c r="J43">
+        <v>0.15448999999999999</v>
+      </c>
+      <c r="K43">
+        <f>J43-I43</f>
+        <v>-3.0230000000000007E-2</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
-        <v>0.15583</v>
+        <v>0.10513</v>
       </c>
       <c r="D44" s="1">
-        <v>0.15583</v>
+        <v>0.10867</v>
       </c>
       <c r="E44">
         <f>D44-C44</f>
-        <v>0</v>
+        <v>3.5400000000000015E-3</v>
+      </c>
+      <c r="I44">
+        <v>0.1711</v>
+      </c>
+      <c r="J44">
+        <v>0.14291999999999999</v>
+      </c>
+      <c r="K44">
+        <f>J44-I44</f>
+        <v>-2.8180000000000011E-2</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
-        <v>0.10513</v>
+        <v>0.22775000000000001</v>
       </c>
       <c r="D45" s="1">
-        <v>0.10867</v>
+        <v>0.23871000000000001</v>
       </c>
       <c r="E45">
         <f>D45-C45</f>
-        <v>3.5400000000000015E-3</v>
+        <v>1.0959999999999998E-2</v>
+      </c>
+      <c r="I45">
+        <v>0.19844999999999999</v>
+      </c>
+      <c r="J45">
+        <v>0.17507</v>
+      </c>
+      <c r="K45">
+        <f>J45-I45</f>
+        <v>-2.3379999999999984E-2</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
-        <v>0.22775000000000001</v>
+        <v>6.9250000000000006E-2</v>
       </c>
       <c r="D46" s="1">
-        <v>0.23871000000000001</v>
+        <v>8.1689999999999999E-2</v>
       </c>
       <c r="E46">
         <f>D46-C46</f>
-        <v>1.0959999999999998E-2</v>
+        <v>1.2439999999999993E-2</v>
+      </c>
+      <c r="I46">
+        <v>0.23177</v>
+      </c>
+      <c r="J46">
+        <v>0.21054</v>
+      </c>
+      <c r="K46">
+        <f>J46-I46</f>
+        <v>-2.1229999999999999E-2</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
-        <v>6.9250000000000006E-2</v>
+        <v>8.5779999999999995E-2</v>
       </c>
       <c r="D47" s="1">
-        <v>8.1689999999999999E-2</v>
+        <v>0.10806</v>
       </c>
       <c r="E47">
         <f>D47-C47</f>
-        <v>1.2439999999999993E-2</v>
+        <v>2.2280000000000008E-2</v>
+      </c>
+      <c r="I47">
+        <v>0.16564000000000001</v>
+      </c>
+      <c r="J47">
+        <v>0.14828</v>
+      </c>
+      <c r="K47">
+        <f>J47-I47</f>
+        <v>-1.7360000000000014E-2</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
-        <v>8.5779999999999995E-2</v>
+        <v>0.10018000000000001</v>
       </c>
       <c r="D48" s="1">
-        <v>0.10806</v>
+        <v>0.12373000000000001</v>
       </c>
       <c r="E48">
         <f>D48-C48</f>
-        <v>2.2280000000000008E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+        <v>2.3550000000000001E-2</v>
+      </c>
+      <c r="I48">
+        <v>0.18423</v>
+      </c>
+      <c r="J48">
+        <v>0.19303000000000001</v>
+      </c>
+      <c r="K48">
+        <f>J48-I48</f>
+        <v>8.8000000000000023E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
-        <v>0.10018000000000001</v>
+        <v>0.10739</v>
       </c>
       <c r="D49" s="1">
-        <v>0.12373000000000001</v>
+        <v>0.13642000000000001</v>
       </c>
       <c r="E49">
         <f>D49-C49</f>
-        <v>2.3550000000000001E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+        <v>2.9030000000000014E-2</v>
+      </c>
+      <c r="I49">
+        <v>0.19505</v>
+      </c>
+      <c r="J49">
+        <v>0.28938999999999998</v>
+      </c>
+      <c r="K49">
+        <f>J49-I49</f>
+        <v>9.4339999999999979E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
-        <v>0.10739</v>
+        <v>3.952E-2</v>
       </c>
       <c r="D50" s="1">
-        <v>0.13642000000000001</v>
+        <v>7.979E-2</v>
       </c>
       <c r="E50">
         <f>D50-C50</f>
-        <v>2.9030000000000014E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+        <v>4.027E-2</v>
+      </c>
+      <c r="I50">
+        <v>0.35672999999999999</v>
+      </c>
+      <c r="J50">
+        <v>0.48531000000000002</v>
+      </c>
+      <c r="K50">
+        <f>J50-I50</f>
+        <v>0.12858000000000003</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
-        <v>3.952E-2</v>
+        <v>0.22552</v>
       </c>
       <c r="D51" s="1">
-        <v>7.979E-2</v>
+        <v>0.66871999999999998</v>
       </c>
       <c r="E51">
         <f>D51-C51</f>
-        <v>4.027E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+        <v>0.44319999999999998</v>
+      </c>
+      <c r="I51">
+        <v>0.30467</v>
+      </c>
+      <c r="J51">
+        <v>0.58159000000000005</v>
+      </c>
+      <c r="K51">
+        <f>J51-I51</f>
+        <v>0.27692000000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
-        <v>0.22552</v>
+        <v>9.4719999999999999E-2</v>
       </c>
       <c r="D52" s="1">
-        <v>0.66871999999999998</v>
+        <v>0.61809000000000003</v>
       </c>
       <c r="E52">
         <f>D52-C52</f>
-        <v>0.44319999999999998</v>
-      </c>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+        <v>0.52337</v>
+      </c>
+      <c r="I52">
+        <v>0.27245000000000003</v>
+      </c>
+      <c r="J52">
+        <v>0.54988000000000004</v>
+      </c>
+      <c r="K52">
+        <f>J52-I52</f>
+        <v>0.27743000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
-        <v>9.4719999999999999E-2</v>
+        <v>0.17169999999999999</v>
       </c>
       <c r="D53" s="1">
-        <v>0.61809000000000003</v>
+        <v>0.7036</v>
       </c>
       <c r="E53">
         <f>D53-C53</f>
-        <v>0.52337</v>
-      </c>
-    </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+        <v>0.53190000000000004</v>
+      </c>
+      <c r="I53">
+        <v>0.13571</v>
+      </c>
+      <c r="J53">
+        <v>0.42720000000000002</v>
+      </c>
+      <c r="K53">
+        <f>J53-I53</f>
+        <v>0.29149000000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
-        <v>0.17169999999999999</v>
+        <v>0.12583</v>
       </c>
       <c r="D54" s="1">
-        <v>0.7036</v>
+        <v>0.72970000000000002</v>
       </c>
       <c r="E54">
         <f>D54-C54</f>
-        <v>0.53190000000000004</v>
-      </c>
-    </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
+        <v>0.60387000000000002</v>
+      </c>
+      <c r="I54">
+        <v>0.13791999999999999</v>
+      </c>
+      <c r="J54">
+        <v>0.50483999999999996</v>
+      </c>
+      <c r="K54">
+        <f>J54-I54</f>
+        <v>0.36691999999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
-        <v>0.12583</v>
+        <v>5.8520000000000003E-2</v>
       </c>
       <c r="D55" s="1">
-        <v>0.72970000000000002</v>
+        <v>0.68994999999999995</v>
       </c>
       <c r="E55">
         <f>D55-C55</f>
-        <v>0.60387000000000002</v>
-      </c>
-    </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+        <v>0.63142999999999994</v>
+      </c>
+      <c r="I55">
+        <v>0.12126000000000001</v>
+      </c>
+      <c r="J55">
+        <v>0.50690999999999997</v>
+      </c>
+      <c r="K55">
+        <f>J55-I55</f>
+        <v>0.38564999999999994</v>
+      </c>
+    </row>
+    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
-        <v>5.8520000000000003E-2</v>
+        <v>0.10376000000000001</v>
       </c>
       <c r="D56" s="1">
-        <v>0.68994999999999995</v>
+        <v>0.76693</v>
       </c>
       <c r="E56">
         <f>D56-C56</f>
-        <v>0.63142999999999994</v>
-      </c>
-    </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+        <v>0.66317000000000004</v>
+      </c>
+      <c r="I56">
+        <v>0.15483</v>
+      </c>
+      <c r="J56">
+        <v>0.56515000000000004</v>
+      </c>
+      <c r="K56">
+        <f>J56-I56</f>
+        <v>0.41032000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
-        <v>0.10376000000000001</v>
+        <v>6.8169999999999994E-2</v>
       </c>
       <c r="D57" s="1">
-        <v>0.76693</v>
+        <v>0.84574000000000005</v>
       </c>
       <c r="E57">
         <f>D57-C57</f>
-        <v>0.66317000000000004</v>
-      </c>
-    </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
+        <v>0.77757000000000009</v>
+      </c>
+      <c r="I57">
+        <v>0.25341000000000002</v>
+      </c>
+      <c r="J57">
+        <v>0.69528000000000001</v>
+      </c>
+      <c r="K57">
+        <f>J57-I57</f>
+        <v>0.44186999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
-        <v>6.8169999999999994E-2</v>
+        <v>0.13325999999999999</v>
       </c>
       <c r="D58" s="1">
-        <v>0.84574000000000005</v>
+        <v>0.99602999999999997</v>
       </c>
       <c r="E58">
         <f>D58-C58</f>
-        <v>0.77757000000000009</v>
-      </c>
-    </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
+        <v>0.86277000000000004</v>
+      </c>
+      <c r="I58">
+        <v>0.42401</v>
+      </c>
+      <c r="J58">
+        <v>0.96660000000000001</v>
+      </c>
+      <c r="K58">
+        <f>J58-I58</f>
+        <v>0.54259000000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
-        <v>0.13325999999999999</v>
+        <v>9.3020000000000005E-2</v>
       </c>
       <c r="D59" s="1">
-        <v>0.99602999999999997</v>
+        <v>1.3063400000000001</v>
       </c>
       <c r="E59">
         <f>D59-C59</f>
-        <v>0.86277000000000004</v>
-      </c>
-    </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
+        <v>1.21332</v>
+      </c>
+      <c r="I59">
+        <v>0.12769</v>
+      </c>
+      <c r="J59">
+        <v>0.8327</v>
+      </c>
+      <c r="K59">
+        <f>J59-I59</f>
+        <v>0.70501000000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
-        <v>9.3020000000000005E-2</v>
+        <v>0.14135</v>
       </c>
       <c r="D60" s="1">
-        <v>1.3063400000000001</v>
+        <v>1.5946400000000001</v>
       </c>
       <c r="E60">
         <f>D60-C60</f>
-        <v>1.21332</v>
-      </c>
-    </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
+        <v>1.45329</v>
+      </c>
+      <c r="I60">
+        <v>0.20893</v>
+      </c>
+      <c r="J60">
+        <v>0.95872999999999997</v>
+      </c>
+      <c r="K60">
+        <f>J60-I60</f>
+        <v>0.74980000000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
-        <v>0.14135</v>
+        <v>8.7379999999999999E-2</v>
       </c>
       <c r="D61" s="1">
-        <v>1.5946400000000001</v>
+        <v>1.6113299999999999</v>
       </c>
       <c r="E61">
         <f>D61-C61</f>
-        <v>1.45329</v>
-      </c>
-    </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
+        <v>1.5239499999999999</v>
+      </c>
+      <c r="I61">
+        <v>0.18040999999999999</v>
+      </c>
+      <c r="J61">
+        <v>1.4315199999999999</v>
+      </c>
+      <c r="K61">
+        <f>J61-I61</f>
+        <v>1.2511099999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
-        <v>8.7379999999999999E-2</v>
+        <v>0.10972</v>
       </c>
       <c r="D62" s="1">
-        <v>1.6113299999999999</v>
+        <v>1.66903</v>
       </c>
       <c r="E62">
         <f>D62-C62</f>
-        <v>1.5239499999999999</v>
-      </c>
-    </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
+        <v>1.55931</v>
+      </c>
+      <c r="I62">
+        <v>0.53849999999999998</v>
+      </c>
+      <c r="J62">
+        <v>2.0443099999999998</v>
+      </c>
+      <c r="K62">
+        <f>J62-I62</f>
+        <v>1.5058099999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
-        <v>0.10972</v>
+        <v>0.10598</v>
       </c>
       <c r="D63" s="1">
-        <v>1.66903</v>
+        <v>1.8714500000000001</v>
       </c>
       <c r="E63">
         <f>D63-C63</f>
-        <v>1.55931</v>
-      </c>
-    </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
+        <v>1.7654700000000001</v>
+      </c>
+      <c r="I63">
+        <v>0.18553</v>
+      </c>
+      <c r="J63">
+        <v>1.82348</v>
+      </c>
+      <c r="K63">
+        <f>J63-I63</f>
+        <v>1.63795</v>
+      </c>
+    </row>
+    <row r="64" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
-        <v>0.10598</v>
+        <v>8.0579999999999999E-2</v>
       </c>
       <c r="D64" s="1">
-        <v>1.8714500000000001</v>
+        <v>1.97102</v>
       </c>
       <c r="E64">
         <f>D64-C64</f>
-        <v>1.7654700000000001</v>
+        <v>1.8904399999999999</v>
+      </c>
+      <c r="I64" t="s">
+        <v>160</v>
+      </c>
+      <c r="K64" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C65" s="1">
-        <v>8.0579999999999999E-2</v>
+        <v>0.16244</v>
       </c>
       <c r="D65" s="1">
-        <v>1.97102</v>
+        <v>2.1956500000000001</v>
       </c>
       <c r="E65">
         <f>D65-C65</f>
-        <v>1.8904399999999999</v>
+        <v>2.03321</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C66" s="1">
-        <v>0.16244</v>
-      </c>
-      <c r="D66" s="1">
-        <v>2.1956500000000001</v>
-      </c>
-      <c r="E66">
-        <f>D66-C66</f>
-        <v>2.03321</v>
+      <c r="C66" t="s">
+        <v>161</v>
+      </c>
+      <c r="E66" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C37:E66">
-    <sortCondition ref="E37:E66"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C36:E66">
+    <sortCondition ref="E66"/>
   </sortState>
   <mergeCells count="8">
     <mergeCell ref="M2:N2"/>
@@ -6895,10 +7218,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:AV34"/>
+  <dimension ref="B1:AV68"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40:D70"/>
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7102,7 +7425,7 @@
       <c r="F4" s="14">
         <v>1174.8499999999999</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="103">
         <f>F4-E4</f>
         <v>-3.875</v>
       </c>
@@ -7204,7 +7527,7 @@
       <c r="F5" s="14">
         <v>1493.0129999999999</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="103">
         <f>F5-E5</f>
         <v>-351.53700000000003</v>
       </c>
@@ -7306,7 +7629,7 @@
       <c r="F6" s="14">
         <v>902.92499999999995</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="103">
         <f>F6-E6</f>
         <v>66.779999999999973</v>
       </c>
@@ -7408,7 +7731,7 @@
       <c r="F7" s="14">
         <v>751.00250000000005</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="103">
         <f>F7-E7</f>
         <v>-17.634999999999991</v>
       </c>
@@ -7510,7 +7833,7 @@
       <c r="F8" s="14">
         <v>736.71</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="103">
         <f>F8-E8</f>
         <v>-41.80499999999995</v>
       </c>
@@ -7612,7 +7935,7 @@
       <c r="F9" s="14">
         <v>891.00250000000005</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="103">
         <f>F9-E9</f>
         <v>31.780000000000086</v>
       </c>
@@ -7690,7 +8013,7 @@
       <c r="F10" s="14">
         <v>812.9425</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="103">
         <f>F10-E10</f>
         <v>-220.36050000000012</v>
       </c>
@@ -7792,7 +8115,7 @@
       <c r="F11" s="14">
         <v>605.76750000000004</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="103">
         <f>F11-E11</f>
         <v>-97.11749999999995</v>
       </c>
@@ -7894,7 +8217,7 @@
       <c r="F12" s="14">
         <v>756.01750000000004</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="103">
         <f>F12-E12</f>
         <v>33.335000000000036</v>
       </c>
@@ -7996,7 +8319,7 @@
       <c r="F13" s="14">
         <v>1523.375</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="103">
         <f>F13-E13</f>
         <v>91.311999999999898</v>
       </c>
@@ -8098,7 +8421,7 @@
       <c r="F14" s="14">
         <v>992.79</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="103">
         <f>F14-E14</f>
         <v>12.302500000000009</v>
       </c>
@@ -8200,7 +8523,7 @@
       <c r="F15" s="14">
         <v>1548.5630000000001</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="103">
         <f>F15-E15</f>
         <v>96.838000000000193</v>
       </c>
@@ -8298,7 +8621,7 @@
       <c r="F16" s="14">
         <v>1666.675</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="103">
         <f>F16-E16</f>
         <v>91.224999999999909</v>
       </c>
@@ -8400,7 +8723,7 @@
       <c r="F17" s="14">
         <v>1328.163</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="103">
         <f>F17-E17</f>
         <v>903.03800000000001</v>
       </c>
@@ -8498,7 +8821,7 @@
       <c r="F18" s="14">
         <v>1338.163</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="103">
         <f>F18-E18</f>
         <v>-7.1369999999999436</v>
       </c>
@@ -8600,7 +8923,7 @@
       <c r="F19" s="14">
         <v>700.70249999999999</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="103">
         <f>F19-E19</f>
         <v>-35.840000000000032</v>
       </c>
@@ -8646,7 +8969,7 @@
       <c r="F20" s="14">
         <v>870.71249999999998</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="103">
         <f>F20-E20</f>
         <v>-865.97550000000012</v>
       </c>
@@ -8748,7 +9071,7 @@
       <c r="F21" s="14">
         <v>904.15250000000003</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="103">
         <f>F21-E21</f>
         <v>-48.522499999999923</v>
       </c>
@@ -8850,7 +9173,7 @@
       <c r="F22" s="14">
         <v>4909.6000000000004</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="103">
         <f>F22-E22</f>
         <v>-24.974999999999454</v>
       </c>
@@ -8952,7 +9275,7 @@
       <c r="F23" s="14">
         <v>1262.875</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="103">
         <f>F23-E23</f>
         <v>90.336999999999989</v>
       </c>
@@ -9054,7 +9377,7 @@
       <c r="F24" s="14">
         <v>899.83</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="103">
         <f>F24-E24</f>
         <v>-28.399999999999977</v>
       </c>
@@ -9156,7 +9479,7 @@
       <c r="F25" s="14">
         <v>350.05380000000002</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="103">
         <f>F25-E25</f>
         <v>-107.05619999999999</v>
       </c>
@@ -9234,7 +9557,7 @@
       <c r="F26" s="14">
         <v>760.08</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="103">
         <f>F26-E26</f>
         <v>-17.5625</v>
       </c>
@@ -9336,7 +9659,7 @@
       <c r="F27" s="14">
         <v>701.48</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="103">
         <f>F27-E27</f>
         <v>-101.07249999999999</v>
       </c>
@@ -9438,7 +9761,7 @@
       <c r="F28" s="14">
         <v>593.49</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="103">
         <f>F28-E28</f>
         <v>-47.069999999999936</v>
       </c>
@@ -9540,7 +9863,7 @@
       <c r="F29" s="14">
         <v>1148.8130000000001</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="103">
         <f>F29-E29</f>
         <v>-284.91199999999981</v>
       </c>
@@ -9642,7 +9965,7 @@
       <c r="F30" s="14">
         <v>1377.125</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="103">
         <f>F30-E30</f>
         <v>-455.02500000000009</v>
       </c>
@@ -9744,7 +10067,7 @@
       <c r="F31" s="14">
         <v>5877.5249999999996</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="103">
         <f>F31-E31</f>
         <v>-190.07500000000073</v>
       </c>
@@ -9846,7 +10169,7 @@
       <c r="F32" s="14">
         <v>718.65</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="103">
         <f>F32-E32</f>
         <v>-33.555000000000064</v>
       </c>
@@ -9948,7 +10271,7 @@
       <c r="F33" s="14">
         <v>768.73249999999996</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="103">
         <f>F33-E33</f>
         <v>-10.797500000000014</v>
       </c>
@@ -10119,17 +10442,371 @@
         <v>34.49</v>
       </c>
     </row>
+    <row r="39" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="E39" s="14">
+        <v>1178.7249999999999</v>
+      </c>
+      <c r="F39" s="14">
+        <v>1174.8499999999999</v>
+      </c>
+      <c r="G39" s="103">
+        <f>F39-E39</f>
+        <v>-3.875</v>
+      </c>
+    </row>
+    <row r="40" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="E40" s="14">
+        <v>1844.55</v>
+      </c>
+      <c r="F40" s="14">
+        <v>1493.0129999999999</v>
+      </c>
+      <c r="G40" s="103">
+        <f>F40-E40</f>
+        <v>-351.53700000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="E41" s="14">
+        <v>836.14499999999998</v>
+      </c>
+      <c r="F41" s="14">
+        <v>902.92499999999995</v>
+      </c>
+      <c r="G41" s="103">
+        <f>F41-E41</f>
+        <v>66.779999999999973</v>
+      </c>
+    </row>
+    <row r="42" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="E42" s="14">
+        <v>768.63750000000005</v>
+      </c>
+      <c r="F42" s="14">
+        <v>751.00250000000005</v>
+      </c>
+      <c r="G42" s="103">
+        <f>F42-E42</f>
+        <v>-17.634999999999991</v>
+      </c>
+    </row>
+    <row r="43" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="E43" s="14">
+        <v>778.51499999999999</v>
+      </c>
+      <c r="F43" s="14">
+        <v>736.71</v>
+      </c>
+      <c r="G43" s="103">
+        <f>F43-E43</f>
+        <v>-41.80499999999995</v>
+      </c>
+    </row>
+    <row r="44" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="E44" s="14">
+        <v>859.22249999999997</v>
+      </c>
+      <c r="F44" s="14">
+        <v>891.00250000000005</v>
+      </c>
+      <c r="G44" s="103">
+        <f>F44-E44</f>
+        <v>31.780000000000086</v>
+      </c>
+    </row>
+    <row r="45" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="E45" s="14">
+        <v>1033.3030000000001</v>
+      </c>
+      <c r="F45" s="14">
+        <v>812.9425</v>
+      </c>
+      <c r="G45" s="103">
+        <f>F45-E45</f>
+        <v>-220.36050000000012</v>
+      </c>
+    </row>
+    <row r="46" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="E46" s="14">
+        <v>702.88499999999999</v>
+      </c>
+      <c r="F46" s="14">
+        <v>605.76750000000004</v>
+      </c>
+      <c r="G46" s="103">
+        <f>F46-E46</f>
+        <v>-97.11749999999995</v>
+      </c>
+    </row>
+    <row r="47" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="E47" s="14">
+        <v>722.6825</v>
+      </c>
+      <c r="F47" s="14">
+        <v>756.01750000000004</v>
+      </c>
+      <c r="G47" s="103">
+        <f>F47-E47</f>
+        <v>33.335000000000036</v>
+      </c>
+    </row>
+    <row r="48" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="E48" s="14">
+        <v>1432.0630000000001</v>
+      </c>
+      <c r="F48" s="14">
+        <v>1523.375</v>
+      </c>
+      <c r="G48" s="103">
+        <f>F48-E48</f>
+        <v>91.311999999999898</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E49" s="14">
+        <v>980.48749999999995</v>
+      </c>
+      <c r="F49" s="14">
+        <v>992.79</v>
+      </c>
+      <c r="G49" s="103">
+        <f>F49-E49</f>
+        <v>12.302500000000009</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E50" s="14">
+        <v>1451.7249999999999</v>
+      </c>
+      <c r="F50" s="14">
+        <v>1548.5630000000001</v>
+      </c>
+      <c r="G50" s="103">
+        <f>F50-E50</f>
+        <v>96.838000000000193</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E51" s="14">
+        <v>1575.45</v>
+      </c>
+      <c r="F51" s="14">
+        <v>1666.675</v>
+      </c>
+      <c r="G51" s="103">
+        <f>F51-E51</f>
+        <v>91.224999999999909</v>
+      </c>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E52" s="14">
+        <v>425.125</v>
+      </c>
+      <c r="F52" s="14">
+        <v>1328.163</v>
+      </c>
+      <c r="G52" s="103">
+        <f>F52-E52</f>
+        <v>903.03800000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E53" s="14">
+        <v>1345.3</v>
+      </c>
+      <c r="F53" s="14">
+        <v>1338.163</v>
+      </c>
+      <c r="G53" s="103">
+        <f>F53-E53</f>
+        <v>-7.1369999999999436</v>
+      </c>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E54" s="14">
+        <v>736.54250000000002</v>
+      </c>
+      <c r="F54" s="14">
+        <v>700.70249999999999</v>
+      </c>
+      <c r="G54" s="103">
+        <f>F54-E54</f>
+        <v>-35.840000000000032</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E55" s="14">
+        <v>1736.6880000000001</v>
+      </c>
+      <c r="F55" s="14">
+        <v>870.71249999999998</v>
+      </c>
+      <c r="G55" s="103">
+        <f>F55-E55</f>
+        <v>-865.97550000000012</v>
+      </c>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E56" s="14">
+        <v>952.67499999999995</v>
+      </c>
+      <c r="F56" s="14">
+        <v>904.15250000000003</v>
+      </c>
+      <c r="G56" s="103">
+        <f>F56-E56</f>
+        <v>-48.522499999999923</v>
+      </c>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E57" s="14">
+        <v>4934.5749999999998</v>
+      </c>
+      <c r="F57" s="14">
+        <v>4909.6000000000004</v>
+      </c>
+      <c r="G57" s="103">
+        <f>F57-E57</f>
+        <v>-24.974999999999454</v>
+      </c>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E58" s="14">
+        <v>1172.538</v>
+      </c>
+      <c r="F58" s="14">
+        <v>1262.875</v>
+      </c>
+      <c r="G58" s="103">
+        <f>F58-E58</f>
+        <v>90.336999999999989</v>
+      </c>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E59" s="14">
+        <v>928.23</v>
+      </c>
+      <c r="F59" s="14">
+        <v>899.83</v>
+      </c>
+      <c r="G59" s="103">
+        <f>F59-E59</f>
+        <v>-28.399999999999977</v>
+      </c>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E60" s="14">
+        <v>457.11</v>
+      </c>
+      <c r="F60" s="14">
+        <v>350.05380000000002</v>
+      </c>
+      <c r="G60" s="103">
+        <f>F60-E60</f>
+        <v>-107.05619999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E61" s="14">
+        <v>777.64250000000004</v>
+      </c>
+      <c r="F61" s="14">
+        <v>760.08</v>
+      </c>
+      <c r="G61" s="103">
+        <f>F61-E61</f>
+        <v>-17.5625</v>
+      </c>
+    </row>
+    <row r="62" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E62" s="14">
+        <v>802.55250000000001</v>
+      </c>
+      <c r="F62" s="14">
+        <v>701.48</v>
+      </c>
+      <c r="G62" s="103">
+        <f>F62-E62</f>
+        <v>-101.07249999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E63" s="14">
+        <v>640.55999999999995</v>
+      </c>
+      <c r="F63" s="14">
+        <v>593.49</v>
+      </c>
+      <c r="G63" s="103">
+        <f>F63-E63</f>
+        <v>-47.069999999999936</v>
+      </c>
+    </row>
+    <row r="64" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E64" s="14">
+        <v>1433.7249999999999</v>
+      </c>
+      <c r="F64" s="14">
+        <v>1148.8130000000001</v>
+      </c>
+      <c r="G64" s="103">
+        <f>F64-E64</f>
+        <v>-284.91199999999981</v>
+      </c>
+    </row>
+    <row r="65" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E65" s="14">
+        <v>1832.15</v>
+      </c>
+      <c r="F65" s="14">
+        <v>1377.125</v>
+      </c>
+      <c r="G65" s="103">
+        <f>F65-E65</f>
+        <v>-455.02500000000009</v>
+      </c>
+    </row>
+    <row r="66" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E66" s="14">
+        <v>6067.6</v>
+      </c>
+      <c r="F66" s="14">
+        <v>5877.5249999999996</v>
+      </c>
+      <c r="G66" s="103">
+        <f>F66-E66</f>
+        <v>-190.07500000000073</v>
+      </c>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E67" s="14">
+        <v>752.20500000000004</v>
+      </c>
+      <c r="F67" s="14">
+        <v>718.65</v>
+      </c>
+      <c r="G67" s="103">
+        <f>F67-E67</f>
+        <v>-33.555000000000064</v>
+      </c>
+    </row>
+    <row r="68" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E68" s="14">
+        <v>779.53</v>
+      </c>
+      <c r="F68" s="14">
+        <v>768.73249999999996</v>
+      </c>
+      <c r="G68" s="103">
+        <f>F68-E68</f>
+        <v>-10.797500000000014</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:C33">
-    <sortCondition ref="C4:C33"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:I34">
+    <sortCondition ref="G33"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="E2:F2"/>
     <mergeCell ref="AL2:AM2"/>
     <mergeCell ref="AO2:AP2"/>
     <mergeCell ref="AR2:AS2"/>
@@ -10140,6 +10817,12 @@
     <mergeCell ref="AC2:AD2"/>
     <mergeCell ref="AF2:AG2"/>
     <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10159,16 +10842,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="86" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
     </row>
     <row r="2" spans="1:87" ht="17.25" x14ac:dyDescent="0.25">
       <c r="C2" s="71" t="s">
@@ -10460,7 +11143,7 @@
       </c>
     </row>
     <row r="4" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="84" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -10660,7 +11343,7 @@
       <c r="CI4" s="23"/>
     </row>
     <row r="5" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A5" s="85"/>
+      <c r="A5" s="84"/>
       <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
@@ -10858,7 +11541,7 @@
       <c r="CI5" s="23"/>
     </row>
     <row r="6" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A6" s="85"/>
+      <c r="A6" s="84"/>
       <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
@@ -11056,7 +11739,7 @@
       <c r="CI6" s="23"/>
     </row>
     <row r="7" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A7" s="85"/>
+      <c r="A7" s="84"/>
       <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
@@ -11254,7 +11937,7 @@
       <c r="CI7" s="23"/>
     </row>
     <row r="8" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A8" s="85"/>
+      <c r="A8" s="84"/>
       <c r="B8" s="9" t="s">
         <v>11</v>
       </c>
@@ -11452,7 +12135,7 @@
       <c r="CI8" s="23"/>
     </row>
     <row r="9" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A9" s="85"/>
+      <c r="A9" s="84"/>
       <c r="B9" s="9" t="s">
         <v>12</v>
       </c>
@@ -11650,7 +12333,7 @@
       <c r="CI9" s="23"/>
     </row>
     <row r="10" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A10" s="85"/>
+      <c r="A10" s="84"/>
       <c r="B10" s="9" t="s">
         <v>13</v>
       </c>
@@ -11848,7 +12531,7 @@
       <c r="CI10" s="23"/>
     </row>
     <row r="11" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A11" s="85"/>
+      <c r="A11" s="84"/>
       <c r="B11" s="9" t="s">
         <v>43</v>
       </c>
@@ -12046,7 +12729,7 @@
       <c r="CI11" s="23"/>
     </row>
     <row r="12" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A12" s="85"/>
+      <c r="A12" s="84"/>
       <c r="B12" s="9" t="s">
         <v>14</v>
       </c>
@@ -12244,7 +12927,7 @@
       <c r="CI12" s="23"/>
     </row>
     <row r="13" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A13" s="85"/>
+      <c r="A13" s="84"/>
       <c r="B13" s="9" t="s">
         <v>15</v>
       </c>
@@ -12442,7 +13125,7 @@
       <c r="CI13" s="23"/>
     </row>
     <row r="14" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A14" s="85"/>
+      <c r="A14" s="84"/>
       <c r="B14" s="9" t="s">
         <v>16</v>
       </c>
@@ -12528,7 +13211,7 @@
       <c r="CI14" s="23"/>
     </row>
     <row r="15" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A15" s="85"/>
+      <c r="A15" s="84"/>
       <c r="B15" s="9" t="s">
         <v>17</v>
       </c>
@@ -12726,7 +13409,7 @@
       <c r="CI15" s="23"/>
     </row>
     <row r="16" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A16" s="85"/>
+      <c r="A16" s="84"/>
       <c r="B16" s="9" t="s">
         <v>18</v>
       </c>
@@ -12924,7 +13607,7 @@
       <c r="CI16" s="23"/>
     </row>
     <row r="17" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A17" s="85"/>
+      <c r="A17" s="84"/>
       <c r="B17" s="9" t="s">
         <v>19</v>
       </c>
@@ -13122,7 +13805,7 @@
       <c r="CI17" s="23"/>
     </row>
     <row r="18" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A18" s="85"/>
+      <c r="A18" s="84"/>
       <c r="B18" s="9" t="s">
         <v>20</v>
       </c>
@@ -13403,7 +14086,7 @@
       <c r="CI19" s="23"/>
     </row>
     <row r="20" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A20" s="86" t="s">
+      <c r="A20" s="85" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="9" t="s">
@@ -13600,7 +14283,7 @@
       </c>
     </row>
     <row r="21" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A21" s="86"/>
+      <c r="A21" s="85"/>
       <c r="B21" s="9" t="s">
         <v>21</v>
       </c>
@@ -13795,7 +14478,7 @@
       </c>
     </row>
     <row r="22" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A22" s="86"/>
+      <c r="A22" s="85"/>
       <c r="B22" s="9" t="s">
         <v>22</v>
       </c>
@@ -13990,7 +14673,7 @@
       </c>
     </row>
     <row r="23" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A23" s="86"/>
+      <c r="A23" s="85"/>
       <c r="B23" s="9" t="s">
         <v>42</v>
       </c>
@@ -14073,7 +14756,7 @@
       <c r="CG23" s="8"/>
     </row>
     <row r="24" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A24" s="86"/>
+      <c r="A24" s="85"/>
       <c r="B24" s="9" t="s">
         <v>23</v>
       </c>
@@ -14268,7 +14951,7 @@
       </c>
     </row>
     <row r="25" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A25" s="86"/>
+      <c r="A25" s="85"/>
       <c r="B25" s="9" t="s">
         <v>46</v>
       </c>
@@ -14463,7 +15146,7 @@
       </c>
     </row>
     <row r="26" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A26" s="86"/>
+      <c r="A26" s="85"/>
       <c r="B26" s="9" t="s">
         <v>24</v>
       </c>
@@ -14658,7 +15341,7 @@
       </c>
     </row>
     <row r="27" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A27" s="86"/>
+      <c r="A27" s="85"/>
       <c r="B27" s="9" t="s">
         <v>25</v>
       </c>
@@ -14853,7 +15536,7 @@
       </c>
     </row>
     <row r="28" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A28" s="86"/>
+      <c r="A28" s="85"/>
       <c r="B28" s="9" t="s">
         <v>26</v>
       </c>
@@ -15048,7 +15731,7 @@
       </c>
     </row>
     <row r="29" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A29" s="86"/>
+      <c r="A29" s="85"/>
       <c r="B29" s="9" t="s">
         <v>27</v>
       </c>
@@ -15243,7 +15926,7 @@
       </c>
     </row>
     <row r="30" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A30" s="86"/>
+      <c r="A30" s="85"/>
       <c r="B30" s="9" t="s">
         <v>28</v>
       </c>
@@ -15438,7 +16121,7 @@
       </c>
     </row>
     <row r="31" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A31" s="86"/>
+      <c r="A31" s="85"/>
       <c r="B31" s="9" t="s">
         <v>29</v>
       </c>
@@ -15633,7 +16316,7 @@
       </c>
     </row>
     <row r="32" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A32" s="86"/>
+      <c r="A32" s="85"/>
       <c r="B32" s="9" t="s">
         <v>30</v>
       </c>
@@ -15828,7 +16511,7 @@
       </c>
     </row>
     <row r="33" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A33" s="86"/>
+      <c r="A33" s="85"/>
       <c r="B33" s="9" t="s">
         <v>31</v>
       </c>
@@ -16023,7 +16706,7 @@
       </c>
     </row>
     <row r="34" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A34" s="86"/>
+      <c r="A34" s="85"/>
       <c r="B34" s="9" t="s">
         <v>32</v>
       </c>
@@ -16297,21 +16980,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A4:A18"/>
-    <mergeCell ref="A20:A34"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="AS2:AT2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="CF2:CG2"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="BN2:BO2"/>
@@ -16328,6 +16996,21 @@
     <mergeCell ref="BK2:BL2"/>
     <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="A4:A18"/>
+    <mergeCell ref="A20:A34"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -16348,16 +17031,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="87" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
     </row>
     <row r="2" spans="1:75" ht="17.25" x14ac:dyDescent="0.25">
       <c r="C2" s="88" t="s">
@@ -16408,26 +17091,26 @@
         <v>83</v>
       </c>
       <c r="AK2" s="88"/>
-      <c r="AM2" s="89" t="s">
+      <c r="AM2" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="AN2" s="89"/>
-      <c r="AP2" s="89" t="s">
+      <c r="AN2" s="90"/>
+      <c r="AP2" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="AQ2" s="89"/>
-      <c r="AS2" s="89" t="s">
+      <c r="AQ2" s="90"/>
+      <c r="AS2" s="90" t="s">
         <v>89</v>
       </c>
-      <c r="AT2" s="89"/>
-      <c r="AV2" s="89" t="s">
+      <c r="AT2" s="90"/>
+      <c r="AV2" s="90" t="s">
         <v>90</v>
       </c>
-      <c r="AW2" s="89"/>
-      <c r="AY2" s="89" t="s">
+      <c r="AW2" s="90"/>
+      <c r="AY2" s="90" t="s">
         <v>91</v>
       </c>
-      <c r="AZ2" s="89"/>
+      <c r="AZ2" s="90"/>
       <c r="BB2" s="88" t="s">
         <v>92</v>
       </c>
@@ -16607,7 +17290,7 @@
       </c>
     </row>
     <row r="4" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="89" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -16762,7 +17445,7 @@
       <c r="BW4" s="25"/>
     </row>
     <row r="5" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A5" s="87"/>
+      <c r="A5" s="89"/>
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
@@ -16915,7 +17598,7 @@
       <c r="BW5" s="25"/>
     </row>
     <row r="6" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A6" s="87"/>
+      <c r="A6" s="89"/>
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
@@ -17068,7 +17751,7 @@
       <c r="BW6" s="25"/>
     </row>
     <row r="7" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A7" s="87"/>
+      <c r="A7" s="89"/>
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
@@ -17221,7 +17904,7 @@
       <c r="BW7" s="25"/>
     </row>
     <row r="8" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A8" s="87"/>
+      <c r="A8" s="89"/>
       <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
@@ -17374,7 +18057,7 @@
       <c r="BW8" s="25"/>
     </row>
     <row r="9" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A9" s="87"/>
+      <c r="A9" s="89"/>
       <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
@@ -17527,7 +18210,7 @@
       <c r="BW9" s="25"/>
     </row>
     <row r="10" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A10" s="87"/>
+      <c r="A10" s="89"/>
       <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
@@ -17680,7 +18363,7 @@
       <c r="BW10" s="25"/>
     </row>
     <row r="11" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A11" s="87"/>
+      <c r="A11" s="89"/>
       <c r="B11" s="7" t="s">
         <v>43</v>
       </c>
@@ -17833,7 +18516,7 @@
       <c r="BW11" s="25"/>
     </row>
     <row r="12" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A12" s="87"/>
+      <c r="A12" s="89"/>
       <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
@@ -17986,7 +18669,7 @@
       <c r="BW12" s="25"/>
     </row>
     <row r="13" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A13" s="87"/>
+      <c r="A13" s="89"/>
       <c r="B13" s="7" t="s">
         <v>15</v>
       </c>
@@ -18139,7 +18822,7 @@
       <c r="BW13" s="25"/>
     </row>
     <row r="14" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A14" s="87"/>
+      <c r="A14" s="89"/>
       <c r="B14" s="7" t="s">
         <v>16</v>
       </c>
@@ -18292,7 +18975,7 @@
       <c r="BW14" s="25"/>
     </row>
     <row r="15" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A15" s="87"/>
+      <c r="A15" s="89"/>
       <c r="B15" s="7" t="s">
         <v>17</v>
       </c>
@@ -18445,7 +19128,7 @@
       <c r="BW15" s="25"/>
     </row>
     <row r="16" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A16" s="87"/>
+      <c r="A16" s="89"/>
       <c r="B16" s="7" t="s">
         <v>18</v>
       </c>
@@ -18598,7 +19281,7 @@
       <c r="BW16" s="25"/>
     </row>
     <row r="17" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A17" s="87"/>
+      <c r="A17" s="89"/>
       <c r="B17" s="7" t="s">
         <v>19</v>
       </c>
@@ -18751,7 +19434,7 @@
       <c r="BW17" s="25"/>
     </row>
     <row r="18" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A18" s="87"/>
+      <c r="A18" s="89"/>
       <c r="B18" s="7" t="s">
         <v>20</v>
       </c>
@@ -18958,7 +19641,7 @@
       <c r="BW19" s="25"/>
     </row>
     <row r="20" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A20" s="87" t="s">
+      <c r="A20" s="89" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -19110,7 +19793,7 @@
       </c>
     </row>
     <row r="21" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A21" s="87"/>
+      <c r="A21" s="89"/>
       <c r="B21" s="7" t="s">
         <v>21</v>
       </c>
@@ -19260,7 +19943,7 @@
       </c>
     </row>
     <row r="22" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A22" s="87"/>
+      <c r="A22" s="89"/>
       <c r="B22" s="7" t="s">
         <v>22</v>
       </c>
@@ -19410,7 +20093,7 @@
       </c>
     </row>
     <row r="23" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A23" s="87"/>
+      <c r="A23" s="89"/>
       <c r="B23" s="7" t="s">
         <v>42</v>
       </c>
@@ -19560,7 +20243,7 @@
       </c>
     </row>
     <row r="24" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A24" s="87"/>
+      <c r="A24" s="89"/>
       <c r="B24" s="7" t="s">
         <v>23</v>
       </c>
@@ -19710,7 +20393,7 @@
       </c>
     </row>
     <row r="25" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A25" s="87"/>
+      <c r="A25" s="89"/>
       <c r="B25" s="7" t="s">
         <v>46</v>
       </c>
@@ -19856,7 +20539,7 @@
       </c>
     </row>
     <row r="26" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A26" s="87"/>
+      <c r="A26" s="89"/>
       <c r="B26" s="7" t="s">
         <v>24</v>
       </c>
@@ -20006,7 +20689,7 @@
       </c>
     </row>
     <row r="27" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A27" s="87"/>
+      <c r="A27" s="89"/>
       <c r="B27" s="7" t="s">
         <v>25</v>
       </c>
@@ -20156,7 +20839,7 @@
       </c>
     </row>
     <row r="28" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A28" s="87"/>
+      <c r="A28" s="89"/>
       <c r="B28" s="7" t="s">
         <v>26</v>
       </c>
@@ -20306,7 +20989,7 @@
       </c>
     </row>
     <row r="29" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A29" s="87"/>
+      <c r="A29" s="89"/>
       <c r="B29" s="7" t="s">
         <v>27</v>
       </c>
@@ -20456,7 +21139,7 @@
       </c>
     </row>
     <row r="30" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A30" s="87"/>
+      <c r="A30" s="89"/>
       <c r="B30" s="7" t="s">
         <v>28</v>
       </c>
@@ -20606,7 +21289,7 @@
       </c>
     </row>
     <row r="31" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A31" s="87"/>
+      <c r="A31" s="89"/>
       <c r="B31" s="7" t="s">
         <v>29</v>
       </c>
@@ -20756,7 +21439,7 @@
       </c>
     </row>
     <row r="32" spans="1:75" x14ac:dyDescent="0.25">
-      <c r="A32" s="87"/>
+      <c r="A32" s="89"/>
       <c r="B32" s="7" t="s">
         <v>30</v>
       </c>
@@ -20906,7 +21589,7 @@
       </c>
     </row>
     <row r="33" spans="1:73" x14ac:dyDescent="0.25">
-      <c r="A33" s="87"/>
+      <c r="A33" s="89"/>
       <c r="B33" s="7" t="s">
         <v>31</v>
       </c>
@@ -21056,7 +21739,7 @@
       </c>
     </row>
     <row r="34" spans="1:73" x14ac:dyDescent="0.25">
-      <c r="A34" s="87"/>
+      <c r="A34" s="89"/>
       <c r="B34" s="7" t="s">
         <v>32</v>
       </c>
@@ -21288,11 +21971,12 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="A20:A34"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BK2:BL2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="BQ2:BR2"/>
+    <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="BT2:BU2"/>
     <mergeCell ref="A4:A18"/>
     <mergeCell ref="AP2:AQ2"/>
@@ -21309,12 +21993,11 @@
     <mergeCell ref="U2:V2"/>
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="A20:A34"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BK2:BL2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="BQ2:BR2"/>
-    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="L2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21335,89 +22018,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="96" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="C2" s="70" t="s">
         <v>102</v>
       </c>
       <c r="D2" s="70"/>
-      <c r="F2" s="99" t="s">
+      <c r="F2" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="99"/>
-      <c r="I2" s="94" t="s">
+      <c r="G2" s="95"/>
+      <c r="I2" s="98" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="95"/>
-      <c r="L2" s="96" t="s">
+      <c r="J2" s="99"/>
+      <c r="L2" s="91" t="s">
         <v>105</v>
       </c>
-      <c r="M2" s="97"/>
-      <c r="O2" s="96" t="s">
+      <c r="M2" s="92"/>
+      <c r="O2" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="97"/>
-      <c r="R2" s="96" t="s">
+      <c r="P2" s="92"/>
+      <c r="R2" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="S2" s="97"/>
-      <c r="U2" s="96" t="s">
+      <c r="S2" s="92"/>
+      <c r="U2" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="V2" s="97"/>
-      <c r="X2" s="96" t="s">
+      <c r="V2" s="92"/>
+      <c r="X2" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="Y2" s="97"/>
-      <c r="AA2" s="96" t="s">
+      <c r="Y2" s="92"/>
+      <c r="AA2" s="91" t="s">
         <v>110</v>
       </c>
-      <c r="AB2" s="97"/>
-      <c r="AD2" s="98" t="s">
+      <c r="AB2" s="92"/>
+      <c r="AD2" s="94" t="s">
         <v>111</v>
       </c>
-      <c r="AE2" s="98"/>
-      <c r="AG2" s="96" t="s">
+      <c r="AE2" s="94"/>
+      <c r="AG2" s="91" t="s">
         <v>112</v>
       </c>
-      <c r="AH2" s="97"/>
-      <c r="AJ2" s="96" t="s">
+      <c r="AH2" s="92"/>
+      <c r="AJ2" s="91" t="s">
         <v>113</v>
       </c>
-      <c r="AK2" s="97"/>
-      <c r="AM2" s="96" t="s">
+      <c r="AK2" s="92"/>
+      <c r="AM2" s="91" t="s">
         <v>114</v>
       </c>
-      <c r="AN2" s="97"/>
-      <c r="AP2" s="96" t="s">
+      <c r="AN2" s="92"/>
+      <c r="AP2" s="91" t="s">
         <v>115</v>
       </c>
-      <c r="AQ2" s="97"/>
-      <c r="AS2" s="96" t="s">
+      <c r="AQ2" s="92"/>
+      <c r="AS2" s="91" t="s">
         <v>116</v>
       </c>
-      <c r="AT2" s="97"/>
-      <c r="AV2" s="96" t="s">
+      <c r="AT2" s="92"/>
+      <c r="AV2" s="91" t="s">
         <v>117</v>
       </c>
-      <c r="AW2" s="97"/>
-      <c r="AY2" s="96" t="s">
+      <c r="AW2" s="92"/>
+      <c r="AY2" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="AZ2" s="97"/>
+      <c r="AZ2" s="92"/>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -21528,7 +22211,7 @@
       </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="93" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="29" t="s">
@@ -21638,7 +22321,7 @@
       </c>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A5" s="92"/>
+      <c r="A5" s="93"/>
       <c r="B5" s="29" t="s">
         <v>8</v>
       </c>
@@ -21746,7 +22429,7 @@
       </c>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A6" s="92"/>
+      <c r="A6" s="93"/>
       <c r="B6" s="29" t="s">
         <v>9</v>
       </c>
@@ -21854,7 +22537,7 @@
       </c>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A7" s="92"/>
+      <c r="A7" s="93"/>
       <c r="B7" s="29" t="s">
         <v>10</v>
       </c>
@@ -21962,7 +22645,7 @@
       </c>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A8" s="92"/>
+      <c r="A8" s="93"/>
       <c r="B8" s="29" t="s">
         <v>11</v>
       </c>
@@ -22070,7 +22753,7 @@
       </c>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A9" s="92"/>
+      <c r="A9" s="93"/>
       <c r="B9" s="29" t="s">
         <v>12</v>
       </c>
@@ -22178,7 +22861,7 @@
       </c>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A10" s="92"/>
+      <c r="A10" s="93"/>
       <c r="B10" s="29" t="s">
         <v>13</v>
       </c>
@@ -22286,7 +22969,7 @@
       </c>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A11" s="92"/>
+      <c r="A11" s="93"/>
       <c r="B11" s="29" t="s">
         <v>43</v>
       </c>
@@ -22394,7 +23077,7 @@
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A12" s="92"/>
+      <c r="A12" s="93"/>
       <c r="B12" s="29" t="s">
         <v>14</v>
       </c>
@@ -22502,7 +23185,7 @@
       </c>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A13" s="92"/>
+      <c r="A13" s="93"/>
       <c r="B13" s="29" t="s">
         <v>15</v>
       </c>
@@ -22610,7 +23293,7 @@
       </c>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A14" s="92"/>
+      <c r="A14" s="93"/>
       <c r="B14" s="29" t="s">
         <v>16</v>
       </c>
@@ -22718,7 +23401,7 @@
       </c>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A15" s="92"/>
+      <c r="A15" s="93"/>
       <c r="B15" s="29" t="s">
         <v>17</v>
       </c>
@@ -22826,7 +23509,7 @@
       </c>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A16" s="92"/>
+      <c r="A16" s="93"/>
       <c r="B16" s="29" t="s">
         <v>18</v>
       </c>
@@ -22934,7 +23617,7 @@
       </c>
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A17" s="92"/>
+      <c r="A17" s="93"/>
       <c r="B17" s="29" t="s">
         <v>19</v>
       </c>
@@ -23042,7 +23725,7 @@
       </c>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A18" s="92"/>
+      <c r="A18" s="93"/>
       <c r="B18" s="29" t="s">
         <v>20</v>
       </c>
@@ -23188,7 +23871,7 @@
       <c r="AZ19" s="31"/>
     </row>
     <row r="20" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A20" s="92" t="s">
+      <c r="A20" s="93" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="29" t="s">
@@ -23298,7 +23981,7 @@
       </c>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A21" s="92"/>
+      <c r="A21" s="93"/>
       <c r="B21" s="29" t="s">
         <v>21</v>
       </c>
@@ -23406,7 +24089,7 @@
       </c>
     </row>
     <row r="22" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A22" s="92"/>
+      <c r="A22" s="93"/>
       <c r="B22" s="29" t="s">
         <v>22</v>
       </c>
@@ -23514,7 +24197,7 @@
       </c>
     </row>
     <row r="23" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A23" s="92"/>
+      <c r="A23" s="93"/>
       <c r="B23" s="29" t="s">
         <v>42</v>
       </c>
@@ -23622,7 +24305,7 @@
       </c>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A24" s="92"/>
+      <c r="A24" s="93"/>
       <c r="B24" s="29" t="s">
         <v>23</v>
       </c>
@@ -23662,7 +24345,7 @@
       <c r="AZ24" s="31"/>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A25" s="92"/>
+      <c r="A25" s="93"/>
       <c r="B25" s="29" t="s">
         <v>46</v>
       </c>
@@ -23770,7 +24453,7 @@
       </c>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A26" s="92"/>
+      <c r="A26" s="93"/>
       <c r="B26" s="29" t="s">
         <v>24</v>
       </c>
@@ -23878,7 +24561,7 @@
       </c>
     </row>
     <row r="27" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A27" s="92"/>
+      <c r="A27" s="93"/>
       <c r="B27" s="29" t="s">
         <v>25</v>
       </c>
@@ -23918,7 +24601,7 @@
       <c r="AZ27" s="31"/>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A28" s="92"/>
+      <c r="A28" s="93"/>
       <c r="B28" s="29" t="s">
         <v>26</v>
       </c>
@@ -24026,7 +24709,7 @@
       </c>
     </row>
     <row r="29" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A29" s="92"/>
+      <c r="A29" s="93"/>
       <c r="B29" s="29" t="s">
         <v>27</v>
       </c>
@@ -24134,7 +24817,7 @@
       </c>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A30" s="92"/>
+      <c r="A30" s="93"/>
       <c r="B30" s="29" t="s">
         <v>28</v>
       </c>
@@ -24242,7 +24925,7 @@
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A31" s="92"/>
+      <c r="A31" s="93"/>
       <c r="B31" s="29" t="s">
         <v>29</v>
       </c>
@@ -24350,7 +25033,7 @@
       </c>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A32" s="92"/>
+      <c r="A32" s="93"/>
       <c r="B32" s="29" t="s">
         <v>30</v>
       </c>
@@ -24458,7 +25141,7 @@
       </c>
     </row>
     <row r="33" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A33" s="92"/>
+      <c r="A33" s="93"/>
       <c r="B33" s="29" t="s">
         <v>31</v>
       </c>
@@ -24566,7 +25249,7 @@
       </c>
     </row>
     <row r="34" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A34" s="92"/>
+      <c r="A34" s="93"/>
       <c r="B34" s="29" t="s">
         <v>32</v>
       </c>
@@ -24674,38 +25357,38 @@
       </c>
     </row>
     <row r="38" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A38" s="91" t="s">
+      <c r="A38" s="96" t="s">
         <v>154</v>
       </c>
-      <c r="B38" s="91"/>
-      <c r="C38" s="91"/>
-      <c r="D38" s="91"/>
-      <c r="E38" s="91"/>
-      <c r="F38" s="91"/>
-      <c r="G38" s="91"/>
-      <c r="H38" s="91"/>
-      <c r="I38" s="91"/>
-      <c r="J38" s="91"/>
-      <c r="K38" s="91"/>
-      <c r="L38" s="91"/>
-      <c r="M38" s="91"/>
-      <c r="N38" s="91"/>
-      <c r="O38" s="91"/>
-      <c r="P38" s="91"/>
-      <c r="Q38" s="91"/>
-      <c r="R38" s="91"/>
+      <c r="B38" s="96"/>
+      <c r="C38" s="96"/>
+      <c r="D38" s="96"/>
+      <c r="E38" s="96"/>
+      <c r="F38" s="96"/>
+      <c r="G38" s="96"/>
+      <c r="H38" s="96"/>
+      <c r="I38" s="96"/>
+      <c r="J38" s="96"/>
+      <c r="K38" s="96"/>
+      <c r="L38" s="96"/>
+      <c r="M38" s="96"/>
+      <c r="N38" s="96"/>
+      <c r="O38" s="96"/>
+      <c r="P38" s="96"/>
+      <c r="Q38" s="96"/>
+      <c r="R38" s="96"/>
     </row>
     <row r="39" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="93" t="s">
+      <c r="C39" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="93"/>
-      <c r="E39" s="93" t="s">
+      <c r="D39" s="97"/>
+      <c r="E39" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="93"/>
+      <c r="F39" s="97"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -24734,7 +25417,7 @@
       </c>
     </row>
     <row r="41" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A41" s="92" t="s">
+      <c r="A41" s="93" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="38" t="s">
@@ -24754,7 +25437,7 @@
       </c>
     </row>
     <row r="42" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A42" s="92"/>
+      <c r="A42" s="93"/>
       <c r="B42" s="29" t="s">
         <v>8</v>
       </c>
@@ -24772,7 +25455,7 @@
       </c>
     </row>
     <row r="43" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A43" s="92"/>
+      <c r="A43" s="93"/>
       <c r="B43" s="29" t="s">
         <v>9</v>
       </c>
@@ -24790,7 +25473,7 @@
       </c>
     </row>
     <row r="44" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A44" s="92"/>
+      <c r="A44" s="93"/>
       <c r="B44" s="29" t="s">
         <v>10</v>
       </c>
@@ -24808,7 +25491,7 @@
       </c>
     </row>
     <row r="45" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A45" s="92"/>
+      <c r="A45" s="93"/>
       <c r="B45" s="29" t="s">
         <v>11</v>
       </c>
@@ -24826,7 +25509,7 @@
       </c>
     </row>
     <row r="46" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A46" s="92"/>
+      <c r="A46" s="93"/>
       <c r="B46" s="29" t="s">
         <v>12</v>
       </c>
@@ -24844,7 +25527,7 @@
       </c>
     </row>
     <row r="47" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A47" s="92"/>
+      <c r="A47" s="93"/>
       <c r="B47" s="29" t="s">
         <v>13</v>
       </c>
@@ -24862,7 +25545,7 @@
       </c>
     </row>
     <row r="48" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A48" s="92"/>
+      <c r="A48" s="93"/>
       <c r="B48" s="29" t="s">
         <v>43</v>
       </c>
@@ -24880,7 +25563,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="92"/>
+      <c r="A49" s="93"/>
       <c r="B49" s="29" t="s">
         <v>14</v>
       </c>
@@ -24898,7 +25581,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="92"/>
+      <c r="A50" s="93"/>
       <c r="B50" s="29" t="s">
         <v>15</v>
       </c>
@@ -24916,7 +25599,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="92"/>
+      <c r="A51" s="93"/>
       <c r="B51" s="29" t="s">
         <v>16</v>
       </c>
@@ -24934,7 +25617,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="92"/>
+      <c r="A52" s="93"/>
       <c r="B52" s="29" t="s">
         <v>17</v>
       </c>
@@ -24952,7 +25635,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="92"/>
+      <c r="A53" s="93"/>
       <c r="B53" s="29" t="s">
         <v>18</v>
       </c>
@@ -24970,7 +25653,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="92"/>
+      <c r="A54" s="93"/>
       <c r="B54" s="29" t="s">
         <v>19</v>
       </c>
@@ -24988,7 +25671,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="92"/>
+      <c r="A55" s="93"/>
       <c r="B55" s="37" t="s">
         <v>20</v>
       </c>
@@ -25014,7 +25697,7 @@
       <c r="F56" s="31"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="92" t="s">
+      <c r="A57" s="93" t="s">
         <v>3</v>
       </c>
       <c r="B57" s="38" t="s">
@@ -25034,7 +25717,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="92"/>
+      <c r="A58" s="93"/>
       <c r="B58" s="29" t="s">
         <v>21</v>
       </c>
@@ -25052,7 +25735,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="92"/>
+      <c r="A59" s="93"/>
       <c r="B59" s="29" t="s">
         <v>22</v>
       </c>
@@ -25070,7 +25753,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="92"/>
+      <c r="A60" s="93"/>
       <c r="B60" s="29" t="s">
         <v>42</v>
       </c>
@@ -25088,7 +25771,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="92"/>
+      <c r="A61" s="93"/>
       <c r="B61" s="29" t="s">
         <v>23</v>
       </c>
@@ -25098,7 +25781,7 @@
       <c r="F61" s="31"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="92"/>
+      <c r="A62" s="93"/>
       <c r="B62" s="29" t="s">
         <v>46</v>
       </c>
@@ -25116,7 +25799,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="92"/>
+      <c r="A63" s="93"/>
       <c r="B63" s="29" t="s">
         <v>24</v>
       </c>
@@ -25134,7 +25817,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="92"/>
+      <c r="A64" s="93"/>
       <c r="B64" s="29" t="s">
         <v>25</v>
       </c>
@@ -25144,7 +25827,7 @@
       <c r="F64" s="31"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="92"/>
+      <c r="A65" s="93"/>
       <c r="B65" s="29" t="s">
         <v>26</v>
       </c>
@@ -25162,7 +25845,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="92"/>
+      <c r="A66" s="93"/>
       <c r="B66" s="29" t="s">
         <v>27</v>
       </c>
@@ -25180,7 +25863,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="92"/>
+      <c r="A67" s="93"/>
       <c r="B67" s="29" t="s">
         <v>28</v>
       </c>
@@ -25198,7 +25881,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="92"/>
+      <c r="A68" s="93"/>
       <c r="B68" s="29" t="s">
         <v>29</v>
       </c>
@@ -25216,7 +25899,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="92"/>
+      <c r="A69" s="93"/>
       <c r="B69" s="29" t="s">
         <v>30</v>
       </c>
@@ -25234,7 +25917,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="92"/>
+      <c r="A70" s="93"/>
       <c r="B70" s="29" t="s">
         <v>31</v>
       </c>
@@ -25252,7 +25935,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="92"/>
+      <c r="A71" s="93"/>
       <c r="B71" s="29" t="s">
         <v>32</v>
       </c>
@@ -25271,6 +25954,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A38:R38"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A57:A71"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="R2:S2"/>
     <mergeCell ref="AY2:AZ2"/>
     <mergeCell ref="A4:A18"/>
     <mergeCell ref="A20:A34"/>
@@ -25287,15 +25979,6 @@
     <mergeCell ref="AD2:AE2"/>
     <mergeCell ref="AG2:AH2"/>
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A38:R38"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A57:A71"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="R2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -30735,21 +31418,11 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A4:A18"/>
-    <mergeCell ref="A20:A34"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="U38:V38"/>
-    <mergeCell ref="X38:Y38"/>
-    <mergeCell ref="AA38:AB38"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A73:G73"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="O38:P38"/>
-    <mergeCell ref="A40:A54"/>
-    <mergeCell ref="A56:A70"/>
+    <mergeCell ref="AD74:AE74"/>
+    <mergeCell ref="AG74:AH74"/>
+    <mergeCell ref="AJ74:AK74"/>
+    <mergeCell ref="AM74:AN74"/>
+    <mergeCell ref="AP74:AQ74"/>
     <mergeCell ref="AA74:AB74"/>
     <mergeCell ref="A76:A90"/>
     <mergeCell ref="A92:A106"/>
@@ -30761,11 +31434,21 @@
     <mergeCell ref="R74:S74"/>
     <mergeCell ref="U74:V74"/>
     <mergeCell ref="X74:Y74"/>
-    <mergeCell ref="AD74:AE74"/>
-    <mergeCell ref="AG74:AH74"/>
-    <mergeCell ref="AJ74:AK74"/>
-    <mergeCell ref="AM74:AN74"/>
-    <mergeCell ref="AP74:AQ74"/>
+    <mergeCell ref="AA38:AB38"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A73:G73"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="A40:A54"/>
+    <mergeCell ref="A56:A70"/>
+    <mergeCell ref="A4:A18"/>
+    <mergeCell ref="A20:A34"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="U38:V38"/>
+    <mergeCell ref="X38:Y38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>